<commit_message>
fix: sub sheet line index used by main sheet
</commit_message>
<xml_diff>
--- a/e1.xlsx
+++ b/e1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\excel-compare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7F1E51-DF55-4AD8-BB43-778E88035F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E56B9E-0E67-4074-919B-A9548984A118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="13546" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>系统名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -184,6 +184,26 @@
   </si>
   <si>
     <t>CABC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ABC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BBC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -761,10 +781,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C1ED27-6622-4C3F-9A5F-289FFE36F446}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -825,6 +845,45 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5">
+        <v>10.1</v>
+      </c>
+      <c r="D5">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6">
+        <v>10.1</v>
+      </c>
+      <c r="D6">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>